<commit_message>
điểm lần 1 (30/12)
</commit_message>
<xml_diff>
--- a/DSSV/pttk_ht_ds.xlsx
+++ b/DSSV/pttk_ht_ds.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyenbangoc\Desktop\me\2013HK1\2k6hk1\2k6hk1\PTTKHT\DSSV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8010" activeTab="1"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="344">
   <si>
     <t>AB</t>
   </si>
@@ -1042,6 +1047,12 @@
   </si>
   <si>
     <t>(*) Hết 16/12-nộp bản mềm bao cao, chậm một ngày - trừ 1 điểm</t>
+  </si>
+  <si>
+    <t>19/12/2016</t>
+  </si>
+  <si>
+    <t>(vắng)</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1063,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1060,14 +1071,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1109,6 +1120,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1157,7 +1171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1192,7 +1206,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1407,19 +1421,19 @@
       <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G1" s="5">
         <v>42702</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,7 +1518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1618,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1788,7 +1802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1873,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +1943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1956,7 +1970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +1999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2207,7 +2221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +2279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2294,7 +2308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +2393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2408,7 +2422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -2466,7 +2480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2553,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -2582,7 +2596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +2623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2692,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +2762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -2775,7 +2789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -2829,7 +2843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -2856,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2885,7 +2899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -2914,7 +2928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2943,7 +2957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -2970,7 +2984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -2997,7 +3011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -3026,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -3055,7 +3069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -3082,7 +3096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -3111,7 +3125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -3140,7 +3154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -3167,7 +3181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -3196,7 +3210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -3223,7 +3237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -3252,7 +3266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -3279,7 +3293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -3306,7 +3320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -3333,7 +3347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -3360,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -3387,7 +3401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -3414,7 +3428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -3441,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -3470,7 +3484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -3499,7 +3513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -3526,7 +3540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -3555,7 +3569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -3582,7 +3596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -3611,7 +3625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -3638,7 +3652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -3667,7 +3681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -3696,7 +3710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -3725,7 +3739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -3752,7 +3766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -3779,7 +3793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -3808,7 +3822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -3837,7 +3851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -3866,7 +3880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -3893,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -3922,7 +3936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -3951,7 +3965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
@@ -3980,7 +3994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -4007,7 +4021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -4063,7 +4077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -4090,7 +4104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -4119,7 +4133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -4148,7 +4162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -4177,7 +4191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -4204,7 +4218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -4233,7 +4247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -4260,7 +4274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -4289,7 +4303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -4316,7 +4330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -4343,7 +4357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -4399,7 +4413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -4426,7 +4440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -4455,7 +4469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -4484,7 +4498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -4513,7 +4527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
@@ -4542,7 +4556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -4571,7 +4585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -4600,7 +4614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -4627,7 +4641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -4654,7 +4668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -4681,7 +4695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -4710,7 +4724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -4737,7 +4751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -4764,7 +4778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -4793,7 +4807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>0</v>
       </c>
@@ -4822,7 +4836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -4849,7 +4863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
@@ -4878,7 +4892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -4907,7 +4921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -4934,7 +4948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -4961,7 +4975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -4988,7 +5002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -5017,7 +5031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>0</v>
       </c>
@@ -5073,7 +5087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>0</v>
       </c>
@@ -5102,7 +5116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -5131,7 +5145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
@@ -5160,7 +5174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -5187,7 +5201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -5216,7 +5230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -5245,7 +5259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -5274,7 +5288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -5330,7 +5344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -5357,7 +5371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>0</v>
       </c>
@@ -5386,7 +5400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F143" s="1" t="s">
         <v>287</v>
       </c>
@@ -5397,7 +5411,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
     </row>
@@ -5408,399 +5422,425 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" t="s">
         <v>288</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" t="s">
         <v>290</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" t="s">
         <v>294</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="E6">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D9" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="E11">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C14" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="E14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C15" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C16" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D16" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D17" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C18" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="E19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>31</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C20" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C21" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D21" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="E21">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D22" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="E22">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>39</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>40</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D25" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>41</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C26" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="E26">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>42</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D26" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>286</v>
@@ -5809,1631 +5849,1723 @@
         <v>317</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>47</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D29" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>50</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D30" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>51</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D31" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>54</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D32" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>55</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C34" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>57</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D35" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>59</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C36" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D36" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>60</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C37" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D37" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>61</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D38" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>63</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C39" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D39" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>64</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C40" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>65</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C41" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D41" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>68</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C42" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D42" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="E42">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>69</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D43" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="E43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>72</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D44" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="E44">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>73</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C45" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>75</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C46" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D46" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>78</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C47" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D47" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>79</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C48" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D48" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>80</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C49" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D49" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="E49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>81</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C50" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D50" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>82</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C51" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D51" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>85</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C52" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D52" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>87</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C53" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D53" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="E53">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>88</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C54" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D54" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>89</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D55" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>91</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C56" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D56" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>95</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D57" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>97</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C58" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D58" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>98</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C59" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D59" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>100</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C60" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D60" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>101</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C61" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D61" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>102</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C62" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D62" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>106</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C63" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D63" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="E63">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>107</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="C64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D64" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>108</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C65" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D65" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>110</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C66" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D66" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>111</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C67" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D67" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>112</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C68" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D68" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>114</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D69" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>116</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C70" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D70" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="E70">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>117</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="C71" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D71" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>118</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D71" s="3" t="s">
+      <c r="C72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>119</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C73" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D73" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="E73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>120</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C74" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D74" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>121</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="C75" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D75" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>122</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="C76" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D76" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="E76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>123</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C77" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D77" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="E77">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>128</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="C78" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>129</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C79" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D79" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="E79">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>130</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="C80" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D80" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="E80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>131</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C81" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="E81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>132</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="C82" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D82" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="E82">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>133</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="C83" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D83" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>137</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="C84" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D84" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>138</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C85" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D85" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>141</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="C86" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D86" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="E86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>142</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C87" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D87" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>2</v>
-      </c>
-      <c r="B87" s="1" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C88" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D88" t="s">
         <v>336</v>
       </c>
-      <c r="E87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>3</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C89" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D89" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="E89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>4</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C90" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D90" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>5</v>
-      </c>
-      <c r="B90" s="1" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C91" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D91" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>7</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C92" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D92" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>10</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C93" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D93" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>11</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C94" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D94" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
         <v>16</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="C95" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D95" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
         <v>17</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C96" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D96" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>21</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C97" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" t="s">
         <v>337</v>
       </c>
-      <c r="E96">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="F97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>26</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C98" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D98" t="s">
         <v>336</v>
       </c>
-      <c r="E97">
+      <c r="F98">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>28</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C99" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D99" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>33</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="C100" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D100" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>34</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="C101" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D101" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
         <v>35</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="C102" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D102" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
         <v>37</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C103" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D103" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
         <v>43</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C104" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D104" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>44</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C105" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D105" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
         <v>45</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="C106" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D106" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
         <v>48</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="C107" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D107" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107">
+      <c r="E107" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
         <v>49</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="C108" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D108" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
         <v>52</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="C109" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D109" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109">
+      <c r="E109" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
         <v>53</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C110" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D110" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>58</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C111" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D111" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111">
+      <c r="E111" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>62</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C112" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D112" t="s">
         <v>336</v>
       </c>
-      <c r="E111">
+      <c r="F112">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
         <v>66</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="C113" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D113" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
         <v>67</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C114" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D114" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
         <v>70</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="C115" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D115" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115">
+      <c r="E115">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
         <v>71</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="C116" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D116" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
         <v>74</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="C117" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D117" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
         <v>76</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="C118" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D118" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
         <v>77</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="C119" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D119" t="s">
         <v>336</v>
       </c>
-      <c r="E118">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119">
+      <c r="F119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
         <v>83</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C120" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D120" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120">
+      <c r="E120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
         <v>84</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="C121" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D121" t="s">
         <v>336</v>
       </c>
-      <c r="E120">
+      <c r="F121">
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
         <v>86</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="C122" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D122" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122">
+      <c r="E122">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
         <v>90</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C123" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D123" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
         <v>92</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C124" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D124" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
         <v>93</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="C125" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D125" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125">
+      <c r="E125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
         <v>94</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="C126" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D126" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
         <v>96</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D126" t="s">
+      <c r="C127" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D127" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
         <v>99</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="C128" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D128" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
         <v>103</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="C129" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D129" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
         <v>104</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D129" s="3" t="s">
+      <c r="C130" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130">
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
         <v>105</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D130" t="s">
+      <c r="C131" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D131" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
         <v>109</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C132" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D132" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
         <v>113</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B133" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D132" t="s">
+      <c r="C133" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D133" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
         <v>115</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D133" t="s">
+      <c r="C134" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D134" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
         <v>124</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D134" t="s">
+      <c r="C135" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D135" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
         <v>125</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D135" t="s">
+      <c r="C136" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D136" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
         <v>126</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D136" t="s">
+      <c r="C137" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D137" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
         <v>127</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D137" t="s">
+      <c r="C138" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D138" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
         <v>134</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D138" t="s">
+      <c r="C139" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D139" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139">
+      <c r="E139" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
         <v>135</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D139" t="s">
+      <c r="C140" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D140" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140">
+      <c r="E140" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
         <v>136</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="C141" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D141" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
         <v>139</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D141" t="s">
+      <c r="C142" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D142" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
         <v>140</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B143" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D142" t="s">
+      <c r="C143" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D143" t="s">
         <v>336</v>
       </c>
     </row>
@@ -7452,7 +7584,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>